<commit_message>
adding all test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_sheet.xlsx
+++ b/src/test/resources/testData/Master_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\OnlineTraining\SeleniumTraining_B15_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1835E0-9AF9-43D1-8E59-C67BF3FD3330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC7B1CA-F77A-429E-8947-828E0D2243C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -212,6 +212,36 @@
   </si>
   <si>
     <t>SignUpPageTitle</t>
+  </si>
+  <si>
+    <t>Functionality_1</t>
+  </si>
+  <si>
+    <t>Functionality_2</t>
+  </si>
+  <si>
+    <t>Functionality_3</t>
+  </si>
+  <si>
+    <t>Functionality_4</t>
+  </si>
+  <si>
+    <t>Functionality_5</t>
+  </si>
+  <si>
+    <t>Functionality_6</t>
+  </si>
+  <si>
+    <t>Functionality_7</t>
+  </si>
+  <si>
+    <t>Functionality_8</t>
+  </si>
+  <si>
+    <t>Functionality_9</t>
+  </si>
+  <si>
+    <t>Functionality_10</t>
   </si>
 </sst>
 </file>
@@ -249,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +295,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -326,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -613,7 +649,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -622,7 +658,7 @@
     <col min="2" max="2" width="17.81640625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.54296875" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -638,7 +674,7 @@
       <c r="D1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>58</v>
       </c>
     </row>
@@ -655,6 +691,9 @@
       <c r="D2" s="11" t="s">
         <v>55</v>
       </c>
+      <c r="E2" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
@@ -669,6 +708,9 @@
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="E3" s="11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
@@ -683,6 +725,9 @@
       <c r="D4" s="11" t="s">
         <v>57</v>
       </c>
+      <c r="E4" s="11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
@@ -697,6 +742,9 @@
       <c r="D5" s="11" t="s">
         <v>55</v>
       </c>
+      <c r="E5" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
@@ -711,12 +759,15 @@
       <c r="D6" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="E6" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -724,13 +775,16 @@
       </c>
       <c r="D7" s="11" t="s">
         <v>57</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -738,13 +792,16 @@
       </c>
       <c r="D8" s="11" t="s">
         <v>55</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -752,13 +809,16 @@
       </c>
       <c r="D9" s="11" t="s">
         <v>56</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -766,13 +826,16 @@
       </c>
       <c r="D10" s="11" t="s">
         <v>57</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -780,6 +843,9 @@
       </c>
       <c r="D11" s="11" t="s">
         <v>56</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -799,7 +865,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
commit to check status
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_sheet.xlsx
+++ b/src/test/resources/testData/Master_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\OnlineTraining\SeleniumTraining_B15_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC7B1CA-F77A-429E-8947-828E0D2243C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15627301-A723-4028-9900-5542283395F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -649,7 +649,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,7 +720,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>57</v>

</xml_diff>